<commit_message>
AMEND HAITONG_N ENTRUST DATA IMPORT TEMPLATE
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Entrust/HaiTong_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Entrust/HaiTong_N.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>申报时间</t>
   </si>
@@ -46,15 +46,6 @@
     <t>合同编号</t>
   </si>
   <si>
-    <t>委托日期</t>
-  </si>
-  <si>
-    <t>股东帐户</t>
-  </si>
-  <si>
-    <t>交易市场</t>
-  </si>
-  <si>
     <t>委托子业务</t>
   </si>
   <si>
@@ -76,7 +67,30 @@
     <t>证券中文名</t>
   </si>
   <si>
+    <t>撤消数量</t>
+  </si>
+  <si>
     <t>交易类别</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>保利地产</t>
+  </si>
+  <si>
+    <t>买</t>
+  </si>
+  <si>
+    <t>已成交</t>
+  </si>
+  <si>
+    <t>正常委托</t>
+  </si>
+  <si>
+    <t>波段</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>出错信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +110,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -120,9 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -429,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -460,46 +484,90 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>0.40943287037037041</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600048</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9.74</v>
+      </c>
+      <c r="K2" s="1">
+        <v>9.74</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3963</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>